<commit_message>
Trying to break as much as possible with one commit Rebranded V3D items and text Removed a ton of deprecated services and defunct pipelines
</commit_message>
<xml_diff>
--- a/FlyWorkstationUserList.xlsx
+++ b/FlyWorkstationUserList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -117,9 +117,6 @@
     <t>Christopher Bruns</t>
   </si>
   <si>
-    <t>Gwenneth Card</t>
-  </si>
-  <si>
     <t>Pete Davies</t>
   </si>
   <si>
@@ -247,6 +244,9 @@
   </si>
   <si>
     <t>Charlotte Weaver</t>
+  </si>
+  <si>
+    <t>Gwyneth Card</t>
   </si>
 </sst>
 </file>
@@ -663,7 +663,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -689,7 +689,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -697,41 +697,41 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
         <v>70</v>
       </c>
-      <c r="B4" t="s">
-        <v>71</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -742,10 +742,10 @@
         <v>31</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -753,10 +753,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -764,13 +764,13 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -778,13 +778,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -792,24 +792,24 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
         <v>72</v>
       </c>
-      <c r="B10" t="s">
-        <v>73</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -817,10 +817,10 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -828,13 +828,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -842,27 +842,27 @@
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" t="s">
         <v>68</v>
       </c>
-      <c r="B14" t="s">
-        <v>69</v>
-      </c>
       <c r="C14" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -870,13 +870,13 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -884,10 +884,10 @@
         <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -895,13 +895,13 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -909,13 +909,13 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -923,13 +923,13 @@
         <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -937,13 +937,13 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -951,13 +951,13 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -965,13 +965,13 @@
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -979,13 +979,13 @@
         <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -993,13 +993,13 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1007,13 +1007,13 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1021,27 +1021,27 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1049,13 +1049,13 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1063,13 +1063,13 @@
         <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1077,49 +1077,49 @@
         <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" t="s">
         <v>74</v>
       </c>
-      <c r="B32" t="s">
-        <v>75</v>
-      </c>
       <c r="D32" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" t="s">
         <v>64</v>
       </c>
-      <c r="B33" t="s">
-        <v>65</v>
-      </c>
       <c r="C33" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1127,13 +1127,13 @@
         <v>14</v>
       </c>
       <c r="B34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1141,13 +1141,13 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1155,13 +1155,13 @@
         <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Making sure the latest user file is committed
</commit_message>
<xml_diff>
--- a/FlyWorkstationUserList.xlsx
+++ b/FlyWorkstationUserList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="92">
   <si>
     <t>Login</t>
   </si>
@@ -247,13 +247,61 @@
   </si>
   <si>
     <t>Gwyneth Card</t>
+  </si>
+  <si>
+    <t>Platform</t>
+  </si>
+  <si>
+    <t>Linux</t>
+  </si>
+  <si>
+    <t>Adam Hantman</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Jenn Jeter</t>
+  </si>
+  <si>
+    <t>jeterj</t>
+  </si>
+  <si>
+    <t>hantmana</t>
+  </si>
+  <si>
+    <t>Mac</t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>cardlab</t>
+  </si>
+  <si>
+    <t>Card Lab</t>
+  </si>
+  <si>
+    <t>parvathama</t>
+  </si>
+  <si>
+    <t>Anitha Parvatham</t>
+  </si>
+  <si>
+    <t>leetlab</t>
+  </si>
+  <si>
+    <t>Tzumin Lee Lab</t>
+  </si>
+  <si>
+    <t>Windows</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -285,6 +333,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -303,7 +358,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -311,8 +366,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -323,14 +390,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -660,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -671,11 +753,12 @@
     <col min="1" max="1" width="27.1640625" customWidth="1"/>
     <col min="2" max="2" width="24.1640625" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="37.33203125" customWidth="1"/>
+    <col min="4" max="5" width="28.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="37.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1">
+    <row r="1" spans="1:6" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -689,10 +772,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -705,8 +791,11 @@
       <c r="D2" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -719,8 +808,11 @@
       <c r="D3" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -734,7 +826,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -747,8 +839,11 @@
       <c r="D5" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="E5" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -759,7 +854,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -773,400 +868,542 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+      <c r="C9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+      <c r="C10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
         <v>71</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+      <c r="D12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
+      <c r="C13" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="C14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
+      <c r="C16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
         <v>67</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B17" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
+      <c r="C17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
         <v>22</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B19" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
+      <c r="C19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
         <v>25</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B20" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
+      <c r="C20" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B21" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
+      <c r="C21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B22" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
+      <c r="C22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
         <v>26</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B23" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
+      <c r="C23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
         <v>13</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B24" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
+      <c r="C24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
         <v>16</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B25" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
+      <c r="C25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
         <v>29</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B27" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
+      <c r="C27" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
         <v>12</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B28" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
+      <c r="C28" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
         <v>10</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B29" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
+      <c r="C29" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
         <v>30</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B30" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
+      <c r="C30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
         <v>7</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B31" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
+      <c r="C31" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
         <v>59</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B32" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
+      <c r="C32" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
         <v>28</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B33" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
+      <c r="C33" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
         <v>19</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B34" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
+      <c r="C34" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
         <v>18</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B35" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
+      <c r="C35" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
         <v>66</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B36" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
+      <c r="C36" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
         <v>73</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B37" t="s">
         <v>74</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
+      <c r="D37" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
         <v>63</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B38" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" t="s">
+      <c r="C38" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
         <v>14</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B39" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
+      <c r="C39" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
         <v>8</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B40" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
+      <c r="C40" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
         <v>15</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B41" t="s">
         <v>54</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>60</v>
+      <c r="C41" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E36">
-    <sortCondition ref="A2:A36"/>
+  <sortState ref="A2:F41">
+    <sortCondition ref="A2:A41"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>